<commit_message>
Reading single objects from file,
</commit_message>
<xml_diff>
--- a/tests/data/marsjanie-db.xlsx
+++ b/tests/data/marsjanie-db.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siemi\aProjects\sn\xlsx-import\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243505CC-CBCF-4DBE-AFC4-64DCF2C5CA43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F1543C-AA64-483E-B5CE-9DA46F113F3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="6870" xr2:uid="{7FD3600F-E097-4036-8B30-56EF2F773847}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="6870" activeTab="2" xr2:uid="{7FD3600F-E097-4036-8B30-56EF2F773847}"/>
   </bookViews>
   <sheets>
     <sheet name="szit1" sheetId="1" r:id="rId1"/>
     <sheet name="grupy" sheetId="2" r:id="rId2"/>
+    <sheet name="contact" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Bada danych osobowych MARSJAN</t>
   </si>
@@ -103,6 +104,18 @@
   </si>
   <si>
     <t>grupa</t>
+  </si>
+  <si>
+    <t>Example author</t>
+  </si>
+  <si>
+    <t>Marian</t>
+  </si>
+  <si>
+    <t>Marianacki</t>
+  </si>
+  <si>
+    <t>Pila-wojenna</t>
   </si>
 </sst>
 </file>
@@ -459,13 +472,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5487BEB-B21E-401C-A054-C3E14AF2693B}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +489,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -485,7 +498,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -494,7 +507,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -503,7 +516,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -512,7 +525,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -535,7 +548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -558,7 +571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
@@ -581,7 +594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -604,7 +617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>4</v>
       </c>
@@ -643,9 +656,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -653,7 +666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -661,7 +674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -672,4 +685,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B804507F-9A19-4107-BAF1-A02261730621}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>